<commit_message>
left only -4th schem
</commit_message>
<xml_diff>
--- a/2 course/ElectricalEngineering/3/Calc.xlsx
+++ b/2 course/ElectricalEngineering/3/Calc.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE4DBA2-6877-48CC-AB84-628C6A71D274}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA7C1E2-011C-4D29-AFE6-13119F33A5A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Schem1" sheetId="2" r:id="rId2"/>
     <sheet name="Schem2" sheetId="3" r:id="rId3"/>
     <sheet name="Schem3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sccem4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>U</t>
   </si>
@@ -121,16 +122,92 @@
   </si>
   <si>
     <t>XC*I</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>ZL</t>
+  </si>
+  <si>
+    <t>ZR</t>
+  </si>
+  <si>
+    <t>ZLRR</t>
+  </si>
+  <si>
+    <t>ZI</t>
+  </si>
+  <si>
+    <t>GLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZLR </t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>arctg((BL-Bc)G) * (-1)</t>
+  </si>
+  <si>
+    <t>fiR</t>
+  </si>
+  <si>
+    <t>fiL</t>
+  </si>
+  <si>
+    <t>Zc</t>
+  </si>
+  <si>
+    <t>Zl</t>
+  </si>
+  <si>
+    <t>ZRC</t>
+  </si>
+  <si>
+    <t>GRC</t>
+  </si>
+  <si>
+    <t>ZRCL</t>
+  </si>
+  <si>
+    <t>Zu</t>
+  </si>
+  <si>
+    <t>URC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,15 +254,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +548,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,12 +658,12 @@
       <c r="M3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>3</v>
       </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1510,15 +1589,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2363A128-0D8A-43FB-9D0D-EB47FABF8C16}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1622,7 +1701,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,11 +1711,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1737,12 +1816,372 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C957BA2-09E2-4958-81BC-F5F5AE2B7D64}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <f ca="1">SQRT(IMREAL(B10)^2 +IMAGINARY(B10)^2)</f>
+        <v>7.3080521286455406E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <f ca="1">COMPLEX(Data!M5,0)</f>
+        <v>55</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="str">
+        <f ca="1">COMPLEX(0,Data!P5)</f>
+        <v>55000i</v>
+      </c>
+      <c r="C5" s="4">
+        <f ca="1">DEGREES(IMARGUMENT(B5))</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <f ca="1">COMPLEX(Data!N5,0)</f>
+        <v>45000</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" ref="C6:C9" ca="1" si="0">DEGREES(IMARGUMENT(B6))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="str">
+        <f ca="1">IMDIV(IMSUM(B5,B6),IMPRODUCT(B5,B6))</f>
+        <v>0.0000222222222222222-0.0000181818181818182i</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>-39.289406862500414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <f ca="1">IMDIV(1,B7)</f>
+        <v>26955.4455445544+22054.4554455446i</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>39.289406862500478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="str">
+        <f ca="1">IMSUM(B6,B8)</f>
+        <v>71955.4455445544+22054.4554455446i</v>
+      </c>
+      <c r="C9" s="4">
+        <f ca="1">DEGREES(IMARGUMENT(B9))</f>
+        <v>17.040383205288041</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="str">
+        <f ca="1">IMDIV(1,B5)</f>
+        <v>-0.0000181818181818182i</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <f ca="1">IMDIV(B4,B9)</f>
+        <v>0.000698721730580138-0.000214159292035399i</v>
+      </c>
+      <c r="C10" s="4">
+        <f ca="1">DEGREES(IMARGUMENT(B10))</f>
+        <v>-17.040383205288041</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="str">
+        <f ca="1">IMDIV(1,Schem3!B6)</f>
+        <v>0.0000222222222222222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="str">
+        <f ca="1">IMPRODUCT(B10,B6)</f>
+        <v>31.4424778761062-9.63716814159296i</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="E11">
+        <f ca="1">SQRT(IMREAL(F9)^2 +IMAGINARY(F9)^2)</f>
+        <v>1.8181818181818199E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="str">
+        <f ca="1">IMSUB(B4,B11)</f>
+        <v>23.5575221238938+9.63716814159296i</v>
+      </c>
+      <c r="E12">
+        <f ca="1">SQRT(IMREAL(F10)^2 +IMAGINARY(F10)^2)</f>
+        <v>2.22222222222222E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="str">
+        <f ca="1">IMDIV(B12,B6)</f>
+        <v>0.000523500491642084+0.000214159292035399i</v>
+      </c>
+      <c r="C13">
+        <f ca="1">SQRT(IMREAL(B13)^2 +IMAGINARY(B13)^2)</f>
+        <v>5.6561202879235777E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="str">
+        <f ca="1">IMDIV(B12,B5)</f>
+        <v>0.000175221238938054-0.000428318584070796i</v>
+      </c>
+      <c r="C14">
+        <f ca="1">SQRT(IMREAL(B14)^2 +IMAGINARY(B14)^2)</f>
+        <v>4.6277347810283828E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <f ca="1">DEGREES(IMARGUMENT(B14))+90</f>
+        <v>22.24902365721249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF8E530-CABE-429C-997C-CC5B8F4F526C}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="str">
+        <f ca="1">COMPLEX(Data!M5,0)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <f ca="1">SQRT(IMREAL(F9)^2 +IMAGINARY(F9)^2)</f>
+        <v>6.7674124470229837E-4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="str">
+        <f ca="1">COMPLEX(0,Data!Q5)</f>
+        <v>50000i</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="str">
+        <f ca="1">IMPRODUCT(F5,F9)</f>
+        <v>35.4364191464001+11.3862110788148i</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="str">
+        <f ca="1">COMPLEX(Data!N5,0)</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="str">
+        <f ca="1">IMSUB(F2,C4)</f>
+        <v>19.5635808535999-11.3862110788148i</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="str">
+        <f ca="1">COMPLEX(0,Data!P5)</f>
+        <v>55000i</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="str">
+        <f ca="1">IMDIV(C5,F4)</f>
+        <v>0.000434746241191109-0.000253026912862551i</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="str">
+        <f ca="1">IMDIV(IMSUM(F4,F3),IMPRODUCT(F4,F3))</f>
+        <v>0.0000222222222222222-0.00002i</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="str">
+        <f ca="1">IMDIV(C5,F5)</f>
+        <v>-0.000207022019614815-0.000355701470065453i</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="str">
+        <f ca="1">IMDIV(1,F6)</f>
+        <v>24861.8784530387+22375.6906077348i</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="str">
+        <f ca="1">IMSUM(F7,F5)</f>
+        <v>24861.8784530387+77375.6906077348i</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="str">
+        <f ca="1">IMDIV(F2,Sccem4!F8)</f>
+        <v>0.000207022019614814-0.000644298529934548i</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>